<commit_message>
Update automatico via Actualizar 05-26-2020 16-40-47
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID_HN_CUARENTENA.xlsx
+++ b/datacovidhn/00 DATACOVID_HN_CUARENTENA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\OneDrive\CORONA VIRUS\DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="185" documentId="8_{427060EC-FABC-4689-88EC-9238ABCB544F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADFE72AD-EA59-4F41-91B8-CAF39B0DAC5F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuarentena_HN" sheetId="1" r:id="rId1"/>
@@ -4593,7 +4593,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5223,7 +5223,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5521,11 +5521,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A9:Q307"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G84" workbookViewId="0">
-      <selection activeCell="Q70" sqref="Q70:Q86"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" hidden="1" customWidth="1"/>
@@ -5544,7 +5544,7 @@
     <col min="18" max="18" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="61.15">
+    <row r="10" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -5646,7 +5646,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="61.15">
+    <row r="11" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="61.15">
+    <row r="12" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -5742,7 +5742,7 @@
       </c>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:17" ht="61.15">
+    <row r="13" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="61.15">
+    <row r="14" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="61.15">
+    <row r="15" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="61.15">
+    <row r="16" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -5934,7 +5934,7 @@
       </c>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="61.15">
+    <row r="17" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="61.15">
+    <row r="18" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -6030,7 +6030,7 @@
       </c>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:16" ht="61.15">
+    <row r="19" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:16" ht="61.15">
+    <row r="20" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" ht="61.15">
+    <row r="21" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="1:16" ht="61.15">
+    <row r="22" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" ht="61.15">
+    <row r="23" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" ht="61.15">
+    <row r="24" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -6318,7 +6318,7 @@
       </c>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="1:16" ht="61.15">
+    <row r="25" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:16" ht="61.15">
+    <row r="26" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:16" ht="61.15">
+    <row r="27" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="1:16" ht="61.15">
+    <row r="28" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -6510,7 +6510,7 @@
       </c>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:16" ht="61.15">
+    <row r="29" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="1:16" ht="61.15">
+    <row r="30" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="1:16" ht="61.15">
+    <row r="31" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="1:16" ht="61.15">
+    <row r="32" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:16" ht="61.15">
+    <row r="33" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="1:16" ht="61.15">
+    <row r="34" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" spans="1:16" ht="61.15">
+    <row r="35" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="1:16" ht="61.15">
+    <row r="36" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -6894,7 +6894,7 @@
       </c>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:16" ht="61.15">
+    <row r="37" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:16" ht="61.15">
+    <row r="38" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -6990,7 +6990,7 @@
       </c>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="1:16" ht="61.15">
+    <row r="39" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
@@ -7038,7 +7038,7 @@
       </c>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:16" ht="61.15">
+    <row r="40" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="1:16" ht="61.15">
+    <row r="41" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="1:16" ht="61.15">
+    <row r="42" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -7182,7 +7182,7 @@
       </c>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="1:16" ht="61.15">
+    <row r="43" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -7230,7 +7230,7 @@
       </c>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="1:16" ht="61.15">
+    <row r="44" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" spans="1:16" ht="61.15">
+    <row r="45" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="1:16" ht="61.15">
+    <row r="46" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" spans="1:16" ht="61.15">
+    <row r="47" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -7422,7 +7422,7 @@
       </c>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="1:16" ht="61.15">
+    <row r="48" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -7470,7 +7470,7 @@
       </c>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" spans="1:16" ht="61.15">
+    <row r="49" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" spans="1:16" ht="61.15">
+    <row r="50" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="1:16" ht="61.15">
+    <row r="51" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -7614,7 +7614,7 @@
       </c>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="1:16" ht="61.15">
+    <row r="52" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="1:16" ht="61.15">
+    <row r="53" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -7710,7 +7710,7 @@
       </c>
       <c r="P53" s="5"/>
     </row>
-    <row r="54" spans="1:16" ht="61.15">
+    <row r="54" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -7758,7 +7758,7 @@
       </c>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="1:16" ht="61.15">
+    <row r="55" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="1:16" ht="61.15">
+    <row r="56" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="P56" s="5"/>
     </row>
-    <row r="57" spans="1:16" ht="61.15">
+    <row r="57" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
@@ -7902,7 +7902,7 @@
       </c>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="1:16" ht="61.15">
+    <row r="58" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="P58" s="5"/>
     </row>
-    <row r="59" spans="1:16" ht="61.15">
+    <row r="59" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="P59" s="5"/>
     </row>
-    <row r="60" spans="1:16" ht="61.15">
+    <row r="60" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -8046,7 +8046,7 @@
       </c>
       <c r="P60" s="5"/>
     </row>
-    <row r="61" spans="1:16" ht="61.15">
+    <row r="61" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -8094,7 +8094,7 @@
       </c>
       <c r="P61" s="5"/>
     </row>
-    <row r="62" spans="1:16" ht="61.15">
+    <row r="62" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -8142,7 +8142,7 @@
       </c>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="1:16" ht="61.15">
+    <row r="63" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="P63" s="5"/>
     </row>
-    <row r="64" spans="1:16" ht="61.15">
+    <row r="64" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="1:16" ht="61.15">
+    <row r="65" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
@@ -8286,7 +8286,7 @@
       </c>
       <c r="P65" s="5"/>
     </row>
-    <row r="66" spans="1:16" ht="61.15">
+    <row r="66" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="P66" s="5"/>
     </row>
-    <row r="67" spans="1:16" ht="61.15">
+    <row r="67" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -8382,7 +8382,7 @@
       </c>
       <c r="P67" s="5"/>
     </row>
-    <row r="68" spans="1:16" ht="61.15">
+    <row r="68" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>17</v>
       </c>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="P68" s="5"/>
     </row>
-    <row r="69" spans="1:16" ht="61.15">
+    <row r="69" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>17</v>
       </c>
@@ -8478,7 +8478,7 @@
       </c>
       <c r="P69" s="5"/>
     </row>
-    <row r="70" spans="1:16" ht="61.15">
+    <row r="70" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="P70" s="5"/>
     </row>
-    <row r="71" spans="1:16" ht="61.15">
+    <row r="71" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
@@ -8574,7 +8574,7 @@
       </c>
       <c r="P71" s="5"/>
     </row>
-    <row r="72" spans="1:16" ht="61.15">
+    <row r="72" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -8622,7 +8622,7 @@
       </c>
       <c r="P72" s="5"/>
     </row>
-    <row r="73" spans="1:16" ht="61.15">
+    <row r="73" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="P73" s="5"/>
     </row>
-    <row r="74" spans="1:16" ht="61.15">
+    <row r="74" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>17</v>
       </c>
@@ -8718,7 +8718,7 @@
       </c>
       <c r="P74" s="5"/>
     </row>
-    <row r="75" spans="1:16" ht="61.15">
+    <row r="75" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -8766,7 +8766,7 @@
       </c>
       <c r="P75" s="5"/>
     </row>
-    <row r="76" spans="1:16" ht="61.15">
+    <row r="76" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>17</v>
       </c>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="P76" s="5"/>
     </row>
-    <row r="77" spans="1:16" ht="61.15">
+    <row r="77" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>17</v>
       </c>
@@ -8862,7 +8862,7 @@
       </c>
       <c r="P77" s="5"/>
     </row>
-    <row r="78" spans="1:16" ht="61.15">
+    <row r="78" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>17</v>
       </c>
@@ -8910,7 +8910,7 @@
       </c>
       <c r="P78" s="5"/>
     </row>
-    <row r="79" spans="1:16" ht="61.15">
+    <row r="79" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -8958,7 +8958,7 @@
       </c>
       <c r="P79" s="5"/>
     </row>
-    <row r="80" spans="1:16" ht="61.15">
+    <row r="80" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="P80" s="5"/>
     </row>
-    <row r="81" spans="1:16" ht="61.15">
+    <row r="81" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>17</v>
       </c>
@@ -9054,7 +9054,7 @@
       </c>
       <c r="P81" s="5"/>
     </row>
-    <row r="82" spans="1:16" ht="61.15">
+    <row r="82" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>17</v>
       </c>
@@ -9102,7 +9102,7 @@
       </c>
       <c r="P82" s="5"/>
     </row>
-    <row r="83" spans="1:16" ht="61.15">
+    <row r="83" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>17</v>
       </c>
@@ -9150,7 +9150,7 @@
       </c>
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="1:16" ht="61.15">
+    <row r="84" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
@@ -9198,7 +9198,7 @@
       </c>
       <c r="P84" s="5"/>
     </row>
-    <row r="85" spans="1:16" ht="61.15">
+    <row r="85" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>17</v>
       </c>
@@ -9246,7 +9246,7 @@
       </c>
       <c r="P85" s="5"/>
     </row>
-    <row r="86" spans="1:16" ht="61.15">
+    <row r="86" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>17</v>
       </c>
@@ -9294,7 +9294,7 @@
       </c>
       <c r="P86" s="5"/>
     </row>
-    <row r="87" spans="1:16" ht="61.15">
+    <row r="87" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>17</v>
       </c>
@@ -9342,7 +9342,7 @@
       </c>
       <c r="P87" s="5"/>
     </row>
-    <row r="88" spans="1:16" ht="61.15">
+    <row r="88" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>17</v>
       </c>
@@ -9390,7 +9390,7 @@
       </c>
       <c r="P88" s="5"/>
     </row>
-    <row r="89" spans="1:16" ht="61.15">
+    <row r="89" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>17</v>
       </c>
@@ -9438,7 +9438,7 @@
       </c>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="1:16" ht="61.15">
+    <row r="90" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>17</v>
       </c>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="P90" s="5"/>
     </row>
-    <row r="91" spans="1:16" ht="61.15">
+    <row r="91" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>17</v>
       </c>
@@ -9534,7 +9534,7 @@
       </c>
       <c r="P91" s="5"/>
     </row>
-    <row r="92" spans="1:16" ht="61.15">
+    <row r="92" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>17</v>
       </c>
@@ -9582,7 +9582,7 @@
       </c>
       <c r="P92" s="5"/>
     </row>
-    <row r="93" spans="1:16" ht="61.15">
+    <row r="93" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>17</v>
       </c>
@@ -9630,7 +9630,7 @@
       </c>
       <c r="P93" s="5"/>
     </row>
-    <row r="94" spans="1:16" ht="61.15">
+    <row r="94" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>17</v>
       </c>
@@ -9678,7 +9678,7 @@
       </c>
       <c r="P94" s="5"/>
     </row>
-    <row r="95" spans="1:16" ht="61.15">
+    <row r="95" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>17</v>
       </c>
@@ -9726,7 +9726,7 @@
       </c>
       <c r="P95" s="5"/>
     </row>
-    <row r="96" spans="1:16" ht="61.15">
+    <row r="96" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>17</v>
       </c>
@@ -9774,7 +9774,7 @@
       </c>
       <c r="P96" s="5"/>
     </row>
-    <row r="97" spans="1:16" ht="61.15">
+    <row r="97" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>17</v>
       </c>
@@ -9822,7 +9822,7 @@
       </c>
       <c r="P97" s="5"/>
     </row>
-    <row r="98" spans="1:16" ht="61.15">
+    <row r="98" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>17</v>
       </c>
@@ -9870,7 +9870,7 @@
       </c>
       <c r="P98" s="5"/>
     </row>
-    <row r="99" spans="1:16" ht="61.15">
+    <row r="99" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>17</v>
       </c>
@@ -9918,7 +9918,7 @@
       </c>
       <c r="P99" s="5"/>
     </row>
-    <row r="100" spans="1:16" ht="61.15">
+    <row r="100" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>17</v>
       </c>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="P100" s="5"/>
     </row>
-    <row r="101" spans="1:16" ht="61.15">
+    <row r="101" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>17</v>
       </c>
@@ -10014,7 +10014,7 @@
       </c>
       <c r="P101" s="5"/>
     </row>
-    <row r="102" spans="1:16" ht="61.15">
+    <row r="102" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>17</v>
       </c>
@@ -10062,7 +10062,7 @@
       </c>
       <c r="P102" s="5"/>
     </row>
-    <row r="103" spans="1:16" ht="61.15">
+    <row r="103" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>17</v>
       </c>
@@ -10110,7 +10110,7 @@
       </c>
       <c r="P103" s="5"/>
     </row>
-    <row r="104" spans="1:16" ht="61.15">
+    <row r="104" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>17</v>
       </c>
@@ -10158,7 +10158,7 @@
       </c>
       <c r="P104" s="5"/>
     </row>
-    <row r="105" spans="1:16" ht="61.15">
+    <row r="105" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>17</v>
       </c>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="P105" s="5"/>
     </row>
-    <row r="106" spans="1:16" ht="61.15">
+    <row r="106" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>17</v>
       </c>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="P106" s="5"/>
     </row>
-    <row r="107" spans="1:16" ht="61.15">
+    <row r="107" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -10302,7 +10302,7 @@
       </c>
       <c r="P107" s="5"/>
     </row>
-    <row r="108" spans="1:16" ht="61.15">
+    <row r="108" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>17</v>
       </c>
@@ -10350,7 +10350,7 @@
       </c>
       <c r="P108" s="5"/>
     </row>
-    <row r="109" spans="1:16" ht="61.15">
+    <row r="109" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>17</v>
       </c>
@@ -10398,7 +10398,7 @@
       </c>
       <c r="P109" s="5"/>
     </row>
-    <row r="110" spans="1:16" ht="61.15">
+    <row r="110" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>17</v>
       </c>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="P110" s="5"/>
     </row>
-    <row r="111" spans="1:16" ht="61.15">
+    <row r="111" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>17</v>
       </c>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="P111" s="5"/>
     </row>
-    <row r="112" spans="1:16" ht="61.15">
+    <row r="112" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>17</v>
       </c>
@@ -10542,7 +10542,7 @@
       </c>
       <c r="P112" s="5"/>
     </row>
-    <row r="113" spans="1:16" ht="61.15">
+    <row r="113" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>17</v>
       </c>
@@ -10590,7 +10590,7 @@
       </c>
       <c r="P113" s="5"/>
     </row>
-    <row r="114" spans="1:16" ht="61.15">
+    <row r="114" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>17</v>
       </c>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="P114" s="5"/>
     </row>
-    <row r="115" spans="1:16" ht="61.15">
+    <row r="115" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>17</v>
       </c>
@@ -10686,7 +10686,7 @@
       </c>
       <c r="P115" s="5"/>
     </row>
-    <row r="116" spans="1:16" ht="61.15">
+    <row r="116" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>17</v>
       </c>
@@ -10734,7 +10734,7 @@
       </c>
       <c r="P116" s="5"/>
     </row>
-    <row r="117" spans="1:16" ht="61.15">
+    <row r="117" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>17</v>
       </c>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="P117" s="5"/>
     </row>
-    <row r="118" spans="1:16" ht="61.15">
+    <row r="118" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>17</v>
       </c>
@@ -10830,7 +10830,7 @@
       </c>
       <c r="P118" s="5"/>
     </row>
-    <row r="119" spans="1:16" ht="61.15">
+    <row r="119" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>17</v>
       </c>
@@ -10878,7 +10878,7 @@
       </c>
       <c r="P119" s="5"/>
     </row>
-    <row r="120" spans="1:16" ht="61.15">
+    <row r="120" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>17</v>
       </c>
@@ -10926,7 +10926,7 @@
       </c>
       <c r="P120" s="5"/>
     </row>
-    <row r="121" spans="1:16" ht="61.15">
+    <row r="121" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>17</v>
       </c>
@@ -10974,7 +10974,7 @@
       </c>
       <c r="P121" s="5"/>
     </row>
-    <row r="122" spans="1:16" ht="61.15">
+    <row r="122" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="P122" s="5"/>
     </row>
-    <row r="123" spans="1:16" ht="61.15">
+    <row r="123" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>17</v>
       </c>
@@ -11070,7 +11070,7 @@
       </c>
       <c r="P123" s="5"/>
     </row>
-    <row r="124" spans="1:16" ht="61.15">
+    <row r="124" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>17</v>
       </c>
@@ -11118,7 +11118,7 @@
       </c>
       <c r="P124" s="5"/>
     </row>
-    <row r="125" spans="1:16" ht="61.15">
+    <row r="125" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>17</v>
       </c>
@@ -11166,7 +11166,7 @@
       </c>
       <c r="P125" s="5"/>
     </row>
-    <row r="126" spans="1:16" ht="61.15">
+    <row r="126" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>17</v>
       </c>
@@ -11214,7 +11214,7 @@
       </c>
       <c r="P126" s="5"/>
     </row>
-    <row r="127" spans="1:16" ht="61.15">
+    <row r="127" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>17</v>
       </c>
@@ -11262,7 +11262,7 @@
       </c>
       <c r="P127" s="5"/>
     </row>
-    <row r="128" spans="1:16" ht="61.15">
+    <row r="128" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>17</v>
       </c>
@@ -11310,7 +11310,7 @@
       </c>
       <c r="P128" s="5"/>
     </row>
-    <row r="129" spans="1:16" ht="61.15">
+    <row r="129" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>17</v>
       </c>
@@ -11358,7 +11358,7 @@
       </c>
       <c r="P129" s="5"/>
     </row>
-    <row r="130" spans="1:16" ht="61.15">
+    <row r="130" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>17</v>
       </c>
@@ -11406,7 +11406,7 @@
       </c>
       <c r="P130" s="5"/>
     </row>
-    <row r="131" spans="1:16" ht="61.15">
+    <row r="131" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>17</v>
       </c>
@@ -11454,7 +11454,7 @@
       </c>
       <c r="P131" s="5"/>
     </row>
-    <row r="132" spans="1:16" ht="61.15">
+    <row r="132" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>17</v>
       </c>
@@ -11502,7 +11502,7 @@
       </c>
       <c r="P132" s="5"/>
     </row>
-    <row r="133" spans="1:16" ht="61.15">
+    <row r="133" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>17</v>
       </c>
@@ -11550,7 +11550,7 @@
       </c>
       <c r="P133" s="5"/>
     </row>
-    <row r="134" spans="1:16" ht="61.15">
+    <row r="134" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>17</v>
       </c>
@@ -11598,7 +11598,7 @@
       </c>
       <c r="P134" s="5"/>
     </row>
-    <row r="135" spans="1:16" ht="61.15">
+    <row r="135" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>17</v>
       </c>
@@ -11646,7 +11646,7 @@
       </c>
       <c r="P135" s="5"/>
     </row>
-    <row r="136" spans="1:16" ht="61.15">
+    <row r="136" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>17</v>
       </c>
@@ -11694,7 +11694,7 @@
       </c>
       <c r="P136" s="5"/>
     </row>
-    <row r="137" spans="1:16" ht="61.15">
+    <row r="137" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>17</v>
       </c>
@@ -11742,7 +11742,7 @@
       </c>
       <c r="P137" s="5"/>
     </row>
-    <row r="138" spans="1:16" ht="61.15">
+    <row r="138" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>17</v>
       </c>
@@ -11790,7 +11790,7 @@
       </c>
       <c r="P138" s="5"/>
     </row>
-    <row r="139" spans="1:16" ht="61.15">
+    <row r="139" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>17</v>
       </c>
@@ -11838,7 +11838,7 @@
       </c>
       <c r="P139" s="5"/>
     </row>
-    <row r="140" spans="1:16" ht="61.15">
+    <row r="140" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>17</v>
       </c>
@@ -11886,7 +11886,7 @@
       </c>
       <c r="P140" s="5"/>
     </row>
-    <row r="141" spans="1:16" ht="61.15">
+    <row r="141" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>17</v>
       </c>
@@ -11934,7 +11934,7 @@
       </c>
       <c r="P141" s="5"/>
     </row>
-    <row r="142" spans="1:16" ht="61.15">
+    <row r="142" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>17</v>
       </c>
@@ -11982,7 +11982,7 @@
       </c>
       <c r="P142" s="5"/>
     </row>
-    <row r="143" spans="1:16" ht="61.15">
+    <row r="143" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>17</v>
       </c>
@@ -12030,7 +12030,7 @@
       </c>
       <c r="P143" s="5"/>
     </row>
-    <row r="144" spans="1:16" ht="61.15">
+    <row r="144" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>17</v>
       </c>
@@ -12078,7 +12078,7 @@
       </c>
       <c r="P144" s="5"/>
     </row>
-    <row r="145" spans="1:16" ht="61.15">
+    <row r="145" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>17</v>
       </c>
@@ -12126,7 +12126,7 @@
       </c>
       <c r="P145" s="5"/>
     </row>
-    <row r="146" spans="1:16" ht="61.15">
+    <row r="146" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>17</v>
       </c>
@@ -12174,7 +12174,7 @@
       </c>
       <c r="P146" s="5"/>
     </row>
-    <row r="147" spans="1:16" ht="61.15">
+    <row r="147" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>17</v>
       </c>
@@ -12222,7 +12222,7 @@
       </c>
       <c r="P147" s="5"/>
     </row>
-    <row r="148" spans="1:16" ht="61.15">
+    <row r="148" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>17</v>
       </c>
@@ -12270,7 +12270,7 @@
       </c>
       <c r="P148" s="5"/>
     </row>
-    <row r="149" spans="1:16" ht="61.15">
+    <row r="149" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>17</v>
       </c>
@@ -12318,7 +12318,7 @@
       </c>
       <c r="P149" s="5"/>
     </row>
-    <row r="150" spans="1:16" ht="61.15">
+    <row r="150" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>17</v>
       </c>
@@ -12366,7 +12366,7 @@
       </c>
       <c r="P150" s="5"/>
     </row>
-    <row r="151" spans="1:16" ht="61.15">
+    <row r="151" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>17</v>
       </c>
@@ -12414,7 +12414,7 @@
       </c>
       <c r="P151" s="5"/>
     </row>
-    <row r="152" spans="1:16" ht="61.15">
+    <row r="152" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>17</v>
       </c>
@@ -12462,7 +12462,7 @@
       </c>
       <c r="P152" s="5"/>
     </row>
-    <row r="153" spans="1:16" ht="61.15">
+    <row r="153" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>17</v>
       </c>
@@ -12510,7 +12510,7 @@
       </c>
       <c r="P153" s="5"/>
     </row>
-    <row r="154" spans="1:16" ht="61.15">
+    <row r="154" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>17</v>
       </c>
@@ -12558,7 +12558,7 @@
       </c>
       <c r="P154" s="5"/>
     </row>
-    <row r="155" spans="1:16" ht="61.15">
+    <row r="155" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>17</v>
       </c>
@@ -12606,7 +12606,7 @@
       </c>
       <c r="P155" s="5"/>
     </row>
-    <row r="156" spans="1:16" ht="61.15">
+    <row r="156" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>17</v>
       </c>
@@ -12654,7 +12654,7 @@
       </c>
       <c r="P156" s="5"/>
     </row>
-    <row r="157" spans="1:16" ht="61.15">
+    <row r="157" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>17</v>
       </c>
@@ -12702,7 +12702,7 @@
       </c>
       <c r="P157" s="5"/>
     </row>
-    <row r="158" spans="1:16" ht="61.15">
+    <row r="158" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>17</v>
       </c>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="P158" s="5"/>
     </row>
-    <row r="159" spans="1:16" ht="61.15">
+    <row r="159" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>17</v>
       </c>
@@ -12798,7 +12798,7 @@
       </c>
       <c r="P159" s="5"/>
     </row>
-    <row r="160" spans="1:16" ht="61.15">
+    <row r="160" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>17</v>
       </c>
@@ -12846,7 +12846,7 @@
       </c>
       <c r="P160" s="5"/>
     </row>
-    <row r="161" spans="1:16" ht="61.15">
+    <row r="161" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>17</v>
       </c>
@@ -12894,7 +12894,7 @@
       </c>
       <c r="P161" s="5"/>
     </row>
-    <row r="162" spans="1:16" ht="61.15">
+    <row r="162" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>17</v>
       </c>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="P162" s="5"/>
     </row>
-    <row r="163" spans="1:16" ht="61.15">
+    <row r="163" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>17</v>
       </c>
@@ -12990,7 +12990,7 @@
       </c>
       <c r="P163" s="5"/>
     </row>
-    <row r="164" spans="1:16" ht="61.15">
+    <row r="164" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>17</v>
       </c>
@@ -13038,7 +13038,7 @@
       </c>
       <c r="P164" s="5"/>
     </row>
-    <row r="165" spans="1:16" ht="61.15">
+    <row r="165" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>17</v>
       </c>
@@ -13086,7 +13086,7 @@
       </c>
       <c r="P165" s="5"/>
     </row>
-    <row r="166" spans="1:16" ht="61.15">
+    <row r="166" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>17</v>
       </c>
@@ -13134,7 +13134,7 @@
       </c>
       <c r="P166" s="5"/>
     </row>
-    <row r="167" spans="1:16" ht="61.15">
+    <row r="167" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>17</v>
       </c>
@@ -13182,7 +13182,7 @@
       </c>
       <c r="P167" s="5"/>
     </row>
-    <row r="168" spans="1:16" ht="61.15">
+    <row r="168" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>17</v>
       </c>
@@ -13230,7 +13230,7 @@
       </c>
       <c r="P168" s="5"/>
     </row>
-    <row r="169" spans="1:16" ht="61.15">
+    <row r="169" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>17</v>
       </c>
@@ -13278,7 +13278,7 @@
       </c>
       <c r="P169" s="5"/>
     </row>
-    <row r="170" spans="1:16" ht="61.15">
+    <row r="170" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>17</v>
       </c>
@@ -13326,7 +13326,7 @@
       </c>
       <c r="P170" s="5"/>
     </row>
-    <row r="171" spans="1:16" ht="61.15">
+    <row r="171" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>17</v>
       </c>
@@ -13374,7 +13374,7 @@
       </c>
       <c r="P171" s="5"/>
     </row>
-    <row r="172" spans="1:16" ht="61.15">
+    <row r="172" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>17</v>
       </c>
@@ -13422,7 +13422,7 @@
       </c>
       <c r="P172" s="5"/>
     </row>
-    <row r="173" spans="1:16" ht="61.15">
+    <row r="173" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>17</v>
       </c>
@@ -13470,7 +13470,7 @@
       </c>
       <c r="P173" s="5"/>
     </row>
-    <row r="174" spans="1:16" ht="61.15">
+    <row r="174" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>17</v>
       </c>
@@ -13518,7 +13518,7 @@
       </c>
       <c r="P174" s="5"/>
     </row>
-    <row r="175" spans="1:16" ht="61.15">
+    <row r="175" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>17</v>
       </c>
@@ -13566,7 +13566,7 @@
       </c>
       <c r="P175" s="5"/>
     </row>
-    <row r="176" spans="1:16" ht="61.15">
+    <row r="176" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>17</v>
       </c>
@@ -13614,7 +13614,7 @@
       </c>
       <c r="P176" s="5"/>
     </row>
-    <row r="177" spans="1:16" ht="61.15">
+    <row r="177" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>17</v>
       </c>
@@ -13662,7 +13662,7 @@
       </c>
       <c r="P177" s="5"/>
     </row>
-    <row r="178" spans="1:16" ht="61.15">
+    <row r="178" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>17</v>
       </c>
@@ -13710,7 +13710,7 @@
       </c>
       <c r="P178" s="5"/>
     </row>
-    <row r="179" spans="1:16" ht="61.15">
+    <row r="179" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>17</v>
       </c>
@@ -13758,7 +13758,7 @@
       </c>
       <c r="P179" s="5"/>
     </row>
-    <row r="180" spans="1:16" ht="61.15">
+    <row r="180" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>17</v>
       </c>
@@ -13806,7 +13806,7 @@
       </c>
       <c r="P180" s="5"/>
     </row>
-    <row r="181" spans="1:16" ht="61.15">
+    <row r="181" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>17</v>
       </c>
@@ -13854,7 +13854,7 @@
       </c>
       <c r="P181" s="5"/>
     </row>
-    <row r="182" spans="1:16" ht="61.15">
+    <row r="182" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>17</v>
       </c>
@@ -13902,7 +13902,7 @@
       </c>
       <c r="P182" s="5"/>
     </row>
-    <row r="183" spans="1:16" ht="61.15">
+    <row r="183" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>17</v>
       </c>
@@ -13950,7 +13950,7 @@
       </c>
       <c r="P183" s="5"/>
     </row>
-    <row r="184" spans="1:16" ht="61.15">
+    <row r="184" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>17</v>
       </c>
@@ -13998,7 +13998,7 @@
       </c>
       <c r="P184" s="5"/>
     </row>
-    <row r="185" spans="1:16" ht="61.15">
+    <row r="185" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>17</v>
       </c>
@@ -14046,7 +14046,7 @@
       </c>
       <c r="P185" s="5"/>
     </row>
-    <row r="186" spans="1:16" ht="61.15">
+    <row r="186" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>17</v>
       </c>
@@ -14094,7 +14094,7 @@
       </c>
       <c r="P186" s="5"/>
     </row>
-    <row r="187" spans="1:16" ht="61.15">
+    <row r="187" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>17</v>
       </c>
@@ -14142,7 +14142,7 @@
       </c>
       <c r="P187" s="5"/>
     </row>
-    <row r="188" spans="1:16" ht="61.15">
+    <row r="188" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>17</v>
       </c>
@@ -14190,7 +14190,7 @@
       </c>
       <c r="P188" s="5"/>
     </row>
-    <row r="189" spans="1:16" ht="61.15">
+    <row r="189" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>17</v>
       </c>
@@ -14238,7 +14238,7 @@
       </c>
       <c r="P189" s="5"/>
     </row>
-    <row r="190" spans="1:16" ht="61.15">
+    <row r="190" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>17</v>
       </c>
@@ -14286,7 +14286,7 @@
       </c>
       <c r="P190" s="5"/>
     </row>
-    <row r="191" spans="1:16" ht="61.15">
+    <row r="191" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>17</v>
       </c>
@@ -14334,7 +14334,7 @@
       </c>
       <c r="P191" s="5"/>
     </row>
-    <row r="192" spans="1:16" ht="61.15">
+    <row r="192" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>17</v>
       </c>
@@ -14382,7 +14382,7 @@
       </c>
       <c r="P192" s="5"/>
     </row>
-    <row r="193" spans="1:16" ht="61.15">
+    <row r="193" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>17</v>
       </c>
@@ -14430,7 +14430,7 @@
       </c>
       <c r="P193" s="5"/>
     </row>
-    <row r="194" spans="1:16" ht="61.15">
+    <row r="194" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>17</v>
       </c>
@@ -14478,7 +14478,7 @@
       </c>
       <c r="P194" s="5"/>
     </row>
-    <row r="195" spans="1:16" ht="61.15">
+    <row r="195" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>17</v>
       </c>
@@ -14526,7 +14526,7 @@
       </c>
       <c r="P195" s="5"/>
     </row>
-    <row r="196" spans="1:16" ht="61.15">
+    <row r="196" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>17</v>
       </c>
@@ -14574,7 +14574,7 @@
       </c>
       <c r="P196" s="5"/>
     </row>
-    <row r="197" spans="1:16" ht="61.15">
+    <row r="197" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>17</v>
       </c>
@@ -14622,7 +14622,7 @@
       </c>
       <c r="P197" s="5"/>
     </row>
-    <row r="198" spans="1:16" ht="61.15">
+    <row r="198" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>17</v>
       </c>
@@ -14670,7 +14670,7 @@
       </c>
       <c r="P198" s="5"/>
     </row>
-    <row r="199" spans="1:16" ht="61.15">
+    <row r="199" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>17</v>
       </c>
@@ -14718,7 +14718,7 @@
       </c>
       <c r="P199" s="5"/>
     </row>
-    <row r="200" spans="1:16" ht="61.15">
+    <row r="200" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>17</v>
       </c>
@@ -14766,7 +14766,7 @@
       </c>
       <c r="P200" s="5"/>
     </row>
-    <row r="201" spans="1:16" ht="61.15">
+    <row r="201" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>17</v>
       </c>
@@ -14814,7 +14814,7 @@
       </c>
       <c r="P201" s="5"/>
     </row>
-    <row r="202" spans="1:16" ht="61.15">
+    <row r="202" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>17</v>
       </c>
@@ -14862,7 +14862,7 @@
       </c>
       <c r="P202" s="5"/>
     </row>
-    <row r="203" spans="1:16" ht="61.15">
+    <row r="203" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>17</v>
       </c>
@@ -14910,7 +14910,7 @@
       </c>
       <c r="P203" s="5"/>
     </row>
-    <row r="204" spans="1:16" ht="61.15">
+    <row r="204" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>17</v>
       </c>
@@ -14958,7 +14958,7 @@
       </c>
       <c r="P204" s="5"/>
     </row>
-    <row r="205" spans="1:16" ht="61.15">
+    <row r="205" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>17</v>
       </c>
@@ -15006,7 +15006,7 @@
       </c>
       <c r="P205" s="5"/>
     </row>
-    <row r="206" spans="1:16" ht="61.15">
+    <row r="206" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>17</v>
       </c>
@@ -15054,7 +15054,7 @@
       </c>
       <c r="P206" s="5"/>
     </row>
-    <row r="207" spans="1:16" ht="61.15">
+    <row r="207" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>17</v>
       </c>
@@ -15102,7 +15102,7 @@
       </c>
       <c r="P207" s="5"/>
     </row>
-    <row r="208" spans="1:16" ht="61.15">
+    <row r="208" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>17</v>
       </c>
@@ -15150,7 +15150,7 @@
       </c>
       <c r="P208" s="5"/>
     </row>
-    <row r="209" spans="1:16" ht="61.15">
+    <row r="209" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>17</v>
       </c>
@@ -15198,7 +15198,7 @@
       </c>
       <c r="P209" s="5"/>
     </row>
-    <row r="210" spans="1:16" ht="61.15">
+    <row r="210" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>17</v>
       </c>
@@ -15246,7 +15246,7 @@
       </c>
       <c r="P210" s="5"/>
     </row>
-    <row r="211" spans="1:16" ht="61.15">
+    <row r="211" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>17</v>
       </c>
@@ -15294,7 +15294,7 @@
       </c>
       <c r="P211" s="5"/>
     </row>
-    <row r="212" spans="1:16" ht="61.15">
+    <row r="212" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>17</v>
       </c>
@@ -15342,7 +15342,7 @@
       </c>
       <c r="P212" s="5"/>
     </row>
-    <row r="213" spans="1:16" ht="61.15">
+    <row r="213" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>17</v>
       </c>
@@ -15390,7 +15390,7 @@
       </c>
       <c r="P213" s="5"/>
     </row>
-    <row r="214" spans="1:16" ht="61.15">
+    <row r="214" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>17</v>
       </c>
@@ -15438,7 +15438,7 @@
       </c>
       <c r="P214" s="5"/>
     </row>
-    <row r="215" spans="1:16" ht="61.15">
+    <row r="215" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>17</v>
       </c>
@@ -15486,7 +15486,7 @@
       </c>
       <c r="P215" s="5"/>
     </row>
-    <row r="216" spans="1:16" ht="61.15">
+    <row r="216" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>17</v>
       </c>
@@ -15534,7 +15534,7 @@
       </c>
       <c r="P216" s="5"/>
     </row>
-    <row r="217" spans="1:16" ht="61.15">
+    <row r="217" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>17</v>
       </c>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="P217" s="5"/>
     </row>
-    <row r="218" spans="1:16" ht="61.15">
+    <row r="218" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>17</v>
       </c>
@@ -15630,7 +15630,7 @@
       </c>
       <c r="P218" s="5"/>
     </row>
-    <row r="219" spans="1:16" ht="61.15">
+    <row r="219" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>17</v>
       </c>
@@ -15678,7 +15678,7 @@
       </c>
       <c r="P219" s="5"/>
     </row>
-    <row r="220" spans="1:16" ht="61.15">
+    <row r="220" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>17</v>
       </c>
@@ -15726,7 +15726,7 @@
       </c>
       <c r="P220" s="5"/>
     </row>
-    <row r="221" spans="1:16" ht="61.15">
+    <row r="221" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>17</v>
       </c>
@@ -15774,7 +15774,7 @@
       </c>
       <c r="P221" s="5"/>
     </row>
-    <row r="222" spans="1:16" ht="61.15">
+    <row r="222" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>17</v>
       </c>
@@ -15822,7 +15822,7 @@
       </c>
       <c r="P222" s="5"/>
     </row>
-    <row r="223" spans="1:16" ht="61.15">
+    <row r="223" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>17</v>
       </c>
@@ -15870,7 +15870,7 @@
       </c>
       <c r="P223" s="5"/>
     </row>
-    <row r="224" spans="1:16" ht="61.15">
+    <row r="224" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>17</v>
       </c>
@@ -15918,7 +15918,7 @@
       </c>
       <c r="P224" s="5"/>
     </row>
-    <row r="225" spans="1:16" ht="61.15">
+    <row r="225" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>17</v>
       </c>
@@ -15966,7 +15966,7 @@
       </c>
       <c r="P225" s="5"/>
     </row>
-    <row r="226" spans="1:16" ht="61.15">
+    <row r="226" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>17</v>
       </c>
@@ -16014,7 +16014,7 @@
       </c>
       <c r="P226" s="5"/>
     </row>
-    <row r="227" spans="1:16" ht="61.15">
+    <row r="227" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>17</v>
       </c>
@@ -16062,7 +16062,7 @@
       </c>
       <c r="P227" s="5"/>
     </row>
-    <row r="228" spans="1:16" ht="61.15">
+    <row r="228" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>17</v>
       </c>
@@ -16110,7 +16110,7 @@
       </c>
       <c r="P228" s="5"/>
     </row>
-    <row r="229" spans="1:16" ht="61.15">
+    <row r="229" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>17</v>
       </c>
@@ -16158,7 +16158,7 @@
       </c>
       <c r="P229" s="5"/>
     </row>
-    <row r="230" spans="1:16" ht="61.15">
+    <row r="230" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>17</v>
       </c>
@@ -16206,7 +16206,7 @@
       </c>
       <c r="P230" s="5"/>
     </row>
-    <row r="231" spans="1:16" ht="61.15">
+    <row r="231" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>17</v>
       </c>
@@ -16254,7 +16254,7 @@
       </c>
       <c r="P231" s="5"/>
     </row>
-    <row r="232" spans="1:16" ht="61.15">
+    <row r="232" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>17</v>
       </c>
@@ -16302,7 +16302,7 @@
       </c>
       <c r="P232" s="5"/>
     </row>
-    <row r="233" spans="1:16" ht="61.15">
+    <row r="233" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>17</v>
       </c>
@@ -16350,7 +16350,7 @@
       </c>
       <c r="P233" s="5"/>
     </row>
-    <row r="234" spans="1:16" ht="61.15">
+    <row r="234" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>17</v>
       </c>
@@ -16398,7 +16398,7 @@
       </c>
       <c r="P234" s="5"/>
     </row>
-    <row r="235" spans="1:16" ht="61.15">
+    <row r="235" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>17</v>
       </c>
@@ -16446,7 +16446,7 @@
       </c>
       <c r="P235" s="5"/>
     </row>
-    <row r="236" spans="1:16" ht="61.15">
+    <row r="236" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>17</v>
       </c>
@@ -16494,7 +16494,7 @@
       </c>
       <c r="P236" s="5"/>
     </row>
-    <row r="237" spans="1:16" ht="61.15">
+    <row r="237" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>17</v>
       </c>
@@ -16542,7 +16542,7 @@
       </c>
       <c r="P237" s="5"/>
     </row>
-    <row r="238" spans="1:16" ht="61.15">
+    <row r="238" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>17</v>
       </c>
@@ -16590,7 +16590,7 @@
       </c>
       <c r="P238" s="5"/>
     </row>
-    <row r="239" spans="1:16" ht="61.15">
+    <row r="239" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>17</v>
       </c>
@@ -16638,7 +16638,7 @@
       </c>
       <c r="P239" s="5"/>
     </row>
-    <row r="240" spans="1:16" ht="61.15">
+    <row r="240" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>17</v>
       </c>
@@ -16686,7 +16686,7 @@
       </c>
       <c r="P240" s="5"/>
     </row>
-    <row r="241" spans="1:16" ht="61.15">
+    <row r="241" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>17</v>
       </c>
@@ -16734,7 +16734,7 @@
       </c>
       <c r="P241" s="5"/>
     </row>
-    <row r="242" spans="1:16" ht="61.15">
+    <row r="242" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>17</v>
       </c>
@@ -16782,7 +16782,7 @@
       </c>
       <c r="P242" s="5"/>
     </row>
-    <row r="243" spans="1:16" ht="61.15">
+    <row r="243" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>17</v>
       </c>
@@ -16830,7 +16830,7 @@
       </c>
       <c r="P243" s="5"/>
     </row>
-    <row r="244" spans="1:16" ht="61.15">
+    <row r="244" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>17</v>
       </c>
@@ -16878,7 +16878,7 @@
       </c>
       <c r="P244" s="5"/>
     </row>
-    <row r="245" spans="1:16" ht="61.15">
+    <row r="245" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>17</v>
       </c>
@@ -16926,7 +16926,7 @@
       </c>
       <c r="P245" s="5"/>
     </row>
-    <row r="246" spans="1:16" ht="61.15">
+    <row r="246" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>17</v>
       </c>
@@ -16974,7 +16974,7 @@
       </c>
       <c r="P246" s="5"/>
     </row>
-    <row r="247" spans="1:16" ht="61.15">
+    <row r="247" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>17</v>
       </c>
@@ -17022,7 +17022,7 @@
       </c>
       <c r="P247" s="5"/>
     </row>
-    <row r="248" spans="1:16" ht="61.15">
+    <row r="248" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>17</v>
       </c>
@@ -17070,7 +17070,7 @@
       </c>
       <c r="P248" s="5"/>
     </row>
-    <row r="249" spans="1:16" ht="61.15">
+    <row r="249" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>17</v>
       </c>
@@ -17118,7 +17118,7 @@
       </c>
       <c r="P249" s="5"/>
     </row>
-    <row r="250" spans="1:16" ht="61.15">
+    <row r="250" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>17</v>
       </c>
@@ -17166,7 +17166,7 @@
       </c>
       <c r="P250" s="5"/>
     </row>
-    <row r="251" spans="1:16" ht="61.15">
+    <row r="251" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>17</v>
       </c>
@@ -17214,7 +17214,7 @@
       </c>
       <c r="P251" s="5"/>
     </row>
-    <row r="252" spans="1:16" ht="61.15">
+    <row r="252" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>17</v>
       </c>
@@ -17262,7 +17262,7 @@
       </c>
       <c r="P252" s="5"/>
     </row>
-    <row r="253" spans="1:16" ht="61.15">
+    <row r="253" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>17</v>
       </c>
@@ -17310,7 +17310,7 @@
       </c>
       <c r="P253" s="5"/>
     </row>
-    <row r="254" spans="1:16" ht="61.15">
+    <row r="254" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>17</v>
       </c>
@@ -17358,7 +17358,7 @@
       </c>
       <c r="P254" s="5"/>
     </row>
-    <row r="255" spans="1:16" ht="61.15">
+    <row r="255" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>17</v>
       </c>
@@ -17406,7 +17406,7 @@
       </c>
       <c r="P255" s="5"/>
     </row>
-    <row r="256" spans="1:16" ht="61.15">
+    <row r="256" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>17</v>
       </c>
@@ -17454,7 +17454,7 @@
       </c>
       <c r="P256" s="5"/>
     </row>
-    <row r="257" spans="1:16" ht="61.15">
+    <row r="257" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>17</v>
       </c>
@@ -17502,7 +17502,7 @@
       </c>
       <c r="P257" s="5"/>
     </row>
-    <row r="258" spans="1:16" ht="61.15">
+    <row r="258" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>17</v>
       </c>
@@ -17550,7 +17550,7 @@
       </c>
       <c r="P258" s="5"/>
     </row>
-    <row r="259" spans="1:16" ht="61.15">
+    <row r="259" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>17</v>
       </c>
@@ -17598,7 +17598,7 @@
       </c>
       <c r="P259" s="5"/>
     </row>
-    <row r="260" spans="1:16" ht="61.15">
+    <row r="260" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>17</v>
       </c>
@@ -17646,7 +17646,7 @@
       </c>
       <c r="P260" s="5"/>
     </row>
-    <row r="261" spans="1:16" ht="61.15">
+    <row r="261" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>17</v>
       </c>
@@ -17694,7 +17694,7 @@
       </c>
       <c r="P261" s="5"/>
     </row>
-    <row r="262" spans="1:16" ht="61.15">
+    <row r="262" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>17</v>
       </c>
@@ -17742,7 +17742,7 @@
       </c>
       <c r="P262" s="5"/>
     </row>
-    <row r="263" spans="1:16" ht="61.15">
+    <row r="263" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>17</v>
       </c>
@@ -17790,7 +17790,7 @@
       </c>
       <c r="P263" s="5"/>
     </row>
-    <row r="264" spans="1:16" ht="61.15">
+    <row r="264" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>17</v>
       </c>
@@ -17838,7 +17838,7 @@
       </c>
       <c r="P264" s="5"/>
     </row>
-    <row r="265" spans="1:16" ht="61.15">
+    <row r="265" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>17</v>
       </c>
@@ -17886,7 +17886,7 @@
       </c>
       <c r="P265" s="5"/>
     </row>
-    <row r="266" spans="1:16" ht="61.15">
+    <row r="266" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>17</v>
       </c>
@@ -17934,7 +17934,7 @@
       </c>
       <c r="P266" s="5"/>
     </row>
-    <row r="267" spans="1:16" ht="61.15">
+    <row r="267" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>17</v>
       </c>
@@ -17982,7 +17982,7 @@
       </c>
       <c r="P267" s="5"/>
     </row>
-    <row r="268" spans="1:16" ht="61.15">
+    <row r="268" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>17</v>
       </c>
@@ -18030,7 +18030,7 @@
       </c>
       <c r="P268" s="5"/>
     </row>
-    <row r="269" spans="1:16" ht="61.15">
+    <row r="269" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>17</v>
       </c>
@@ -18078,7 +18078,7 @@
       </c>
       <c r="P269" s="5"/>
     </row>
-    <row r="270" spans="1:16" ht="61.15">
+    <row r="270" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>17</v>
       </c>
@@ -18126,7 +18126,7 @@
       </c>
       <c r="P270" s="5"/>
     </row>
-    <row r="271" spans="1:16" ht="61.15">
+    <row r="271" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>17</v>
       </c>
@@ -18174,7 +18174,7 @@
       </c>
       <c r="P271" s="5"/>
     </row>
-    <row r="272" spans="1:16" ht="61.15">
+    <row r="272" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>17</v>
       </c>
@@ -18222,7 +18222,7 @@
       </c>
       <c r="P272" s="5"/>
     </row>
-    <row r="273" spans="1:16" ht="61.15">
+    <row r="273" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>17</v>
       </c>
@@ -18270,7 +18270,7 @@
       </c>
       <c r="P273" s="5"/>
     </row>
-    <row r="274" spans="1:16" ht="61.15">
+    <row r="274" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>17</v>
       </c>
@@ -18318,7 +18318,7 @@
       </c>
       <c r="P274" s="5"/>
     </row>
-    <row r="275" spans="1:16" ht="61.15">
+    <row r="275" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>17</v>
       </c>
@@ -18366,7 +18366,7 @@
       </c>
       <c r="P275" s="5"/>
     </row>
-    <row r="276" spans="1:16" ht="61.15">
+    <row r="276" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>17</v>
       </c>
@@ -18414,7 +18414,7 @@
       </c>
       <c r="P276" s="5"/>
     </row>
-    <row r="277" spans="1:16" ht="61.15">
+    <row r="277" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>17</v>
       </c>
@@ -18462,7 +18462,7 @@
       </c>
       <c r="P277" s="5"/>
     </row>
-    <row r="278" spans="1:16" ht="61.15">
+    <row r="278" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>17</v>
       </c>
@@ -18510,7 +18510,7 @@
       </c>
       <c r="P278" s="5"/>
     </row>
-    <row r="279" spans="1:16" ht="61.15">
+    <row r="279" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>17</v>
       </c>
@@ -18558,7 +18558,7 @@
       </c>
       <c r="P279" s="5"/>
     </row>
-    <row r="280" spans="1:16" ht="61.15">
+    <row r="280" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>17</v>
       </c>
@@ -18606,7 +18606,7 @@
       </c>
       <c r="P280" s="5"/>
     </row>
-    <row r="281" spans="1:16" ht="61.15">
+    <row r="281" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>17</v>
       </c>
@@ -18654,7 +18654,7 @@
       </c>
       <c r="P281" s="5"/>
     </row>
-    <row r="282" spans="1:16" ht="61.15">
+    <row r="282" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>17</v>
       </c>
@@ -18702,7 +18702,7 @@
       </c>
       <c r="P282" s="5"/>
     </row>
-    <row r="283" spans="1:16" ht="61.15">
+    <row r="283" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>17</v>
       </c>
@@ -18750,7 +18750,7 @@
       </c>
       <c r="P283" s="5"/>
     </row>
-    <row r="284" spans="1:16" ht="61.15">
+    <row r="284" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>17</v>
       </c>
@@ -18798,7 +18798,7 @@
       </c>
       <c r="P284" s="5"/>
     </row>
-    <row r="285" spans="1:16" ht="61.15">
+    <row r="285" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>17</v>
       </c>
@@ -18846,7 +18846,7 @@
       </c>
       <c r="P285" s="5"/>
     </row>
-    <row r="286" spans="1:16" ht="61.15">
+    <row r="286" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>17</v>
       </c>
@@ -18894,7 +18894,7 @@
       </c>
       <c r="P286" s="5"/>
     </row>
-    <row r="287" spans="1:16" ht="61.15">
+    <row r="287" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>17</v>
       </c>
@@ -18942,7 +18942,7 @@
       </c>
       <c r="P287" s="5"/>
     </row>
-    <row r="288" spans="1:16" ht="61.15">
+    <row r="288" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>17</v>
       </c>
@@ -18990,7 +18990,7 @@
       </c>
       <c r="P288" s="5"/>
     </row>
-    <row r="289" spans="1:16" ht="61.15">
+    <row r="289" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>17</v>
       </c>
@@ -19038,7 +19038,7 @@
       </c>
       <c r="P289" s="5"/>
     </row>
-    <row r="290" spans="1:16" ht="61.15">
+    <row r="290" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>17</v>
       </c>
@@ -19086,7 +19086,7 @@
       </c>
       <c r="P290" s="5"/>
     </row>
-    <row r="291" spans="1:16" ht="61.15">
+    <row r="291" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>17</v>
       </c>
@@ -19134,7 +19134,7 @@
       </c>
       <c r="P291" s="5"/>
     </row>
-    <row r="292" spans="1:16" ht="61.15">
+    <row r="292" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>17</v>
       </c>
@@ -19182,7 +19182,7 @@
       </c>
       <c r="P292" s="5"/>
     </row>
-    <row r="293" spans="1:16" ht="61.15">
+    <row r="293" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>17</v>
       </c>
@@ -19230,7 +19230,7 @@
       </c>
       <c r="P293" s="5"/>
     </row>
-    <row r="294" spans="1:16" ht="61.15">
+    <row r="294" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>17</v>
       </c>
@@ -19278,7 +19278,7 @@
       </c>
       <c r="P294" s="5"/>
     </row>
-    <row r="295" spans="1:16" ht="61.15">
+    <row r="295" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>17</v>
       </c>
@@ -19326,7 +19326,7 @@
       </c>
       <c r="P295" s="5"/>
     </row>
-    <row r="296" spans="1:16" ht="61.15">
+    <row r="296" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>17</v>
       </c>
@@ -19374,7 +19374,7 @@
       </c>
       <c r="P296" s="5"/>
     </row>
-    <row r="297" spans="1:16" ht="61.15">
+    <row r="297" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>17</v>
       </c>
@@ -19422,7 +19422,7 @@
       </c>
       <c r="P297" s="5"/>
     </row>
-    <row r="298" spans="1:16" ht="61.15">
+    <row r="298" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>17</v>
       </c>
@@ -19470,7 +19470,7 @@
       </c>
       <c r="P298" s="5"/>
     </row>
-    <row r="299" spans="1:16" ht="61.15">
+    <row r="299" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>17</v>
       </c>
@@ -19518,7 +19518,7 @@
       </c>
       <c r="P299" s="5"/>
     </row>
-    <row r="300" spans="1:16" ht="61.15">
+    <row r="300" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>17</v>
       </c>
@@ -19566,7 +19566,7 @@
       </c>
       <c r="P300" s="5"/>
     </row>
-    <row r="301" spans="1:16" ht="61.15">
+    <row r="301" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>17</v>
       </c>
@@ -19614,7 +19614,7 @@
       </c>
       <c r="P301" s="5"/>
     </row>
-    <row r="302" spans="1:16" ht="61.15">
+    <row r="302" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>17</v>
       </c>
@@ -19662,7 +19662,7 @@
       </c>
       <c r="P302" s="5"/>
     </row>
-    <row r="303" spans="1:16" ht="61.15">
+    <row r="303" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>17</v>
       </c>
@@ -19710,7 +19710,7 @@
       </c>
       <c r="P303" s="5"/>
     </row>
-    <row r="304" spans="1:16" ht="61.15">
+    <row r="304" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>17</v>
       </c>
@@ -19758,7 +19758,7 @@
       </c>
       <c r="P304" s="5"/>
     </row>
-    <row r="305" spans="1:16" ht="61.15">
+    <row r="305" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>17</v>
       </c>
@@ -19806,7 +19806,7 @@
       </c>
       <c r="P305" s="5"/>
     </row>
-    <row r="306" spans="1:16" ht="61.15">
+    <row r="306" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>17</v>
       </c>
@@ -19854,7 +19854,7 @@
       </c>
       <c r="P306" s="5"/>
     </row>
-    <row r="307" spans="1:16" ht="61.15">
+    <row r="307" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-06-2020 16-25-07
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID_HN_CUARENTENA.xlsx
+++ b/datacovidhn/00 DATACOVID_HN_CUARENTENA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\OneDrive\CORONA VIRUS\DATACOVID HN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{427060EC-FABC-4689-88EC-9238ABCB544F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADFE72AD-EA59-4F41-91B8-CAF39B0DAC5F}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="8_{427060EC-FABC-4689-88EC-9238ABCB544F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB51728F-783C-4B41-85E5-180F0825228B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuarentena_HN" sheetId="1" r:id="rId1"/>
@@ -4912,8 +4912,8 @@
       <xdr:rowOff>7621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>830580</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>129541</xdr:rowOff>
     </xdr:to>
@@ -4984,14 +4984,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -5062,14 +5062,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2385060</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>906780</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -5522,29 +5522,29 @@
   <dimension ref="A9:Q307"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="12" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.44140625" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="45.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" customWidth="1"/>
-    <col min="17" max="17" width="33.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="45.5546875" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" customWidth="1"/>
+    <col min="17" max="17" width="33.88671875" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -5646,7 +5646,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -5742,7 +5742,7 @@
       </c>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -5934,7 +5934,7 @@
       </c>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -6030,7 +6030,7 @@
       </c>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -6318,7 +6318,7 @@
       </c>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -6510,7 +6510,7 @@
       </c>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -6894,7 +6894,7 @@
       </c>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -6990,7 +6990,7 @@
       </c>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
@@ -7038,7 +7038,7 @@
       </c>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -7182,7 +7182,7 @@
       </c>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -7230,7 +7230,7 @@
       </c>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -7422,7 +7422,7 @@
       </c>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -7470,7 +7470,7 @@
       </c>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -7614,7 +7614,7 @@
       </c>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -7710,7 +7710,7 @@
       </c>
       <c r="P53" s="5"/>
     </row>
-    <row r="54" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -7758,7 +7758,7 @@
       </c>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="P56" s="5"/>
     </row>
-    <row r="57" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
@@ -7902,7 +7902,7 @@
       </c>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="P58" s="5"/>
     </row>
-    <row r="59" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="P59" s="5"/>
     </row>
-    <row r="60" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -8046,7 +8046,7 @@
       </c>
       <c r="P60" s="5"/>
     </row>
-    <row r="61" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -8094,7 +8094,7 @@
       </c>
       <c r="P61" s="5"/>
     </row>
-    <row r="62" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -8142,7 +8142,7 @@
       </c>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="P63" s="5"/>
     </row>
-    <row r="64" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
@@ -8286,7 +8286,7 @@
       </c>
       <c r="P65" s="5"/>
     </row>
-    <row r="66" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="P66" s="5"/>
     </row>
-    <row r="67" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -8382,7 +8382,7 @@
       </c>
       <c r="P67" s="5"/>
     </row>
-    <row r="68" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>17</v>
       </c>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="P68" s="5"/>
     </row>
-    <row r="69" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>17</v>
       </c>
@@ -8478,7 +8478,7 @@
       </c>
       <c r="P69" s="5"/>
     </row>
-    <row r="70" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="P70" s="5"/>
     </row>
-    <row r="71" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
@@ -8574,7 +8574,7 @@
       </c>
       <c r="P71" s="5"/>
     </row>
-    <row r="72" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -8622,7 +8622,7 @@
       </c>
       <c r="P72" s="5"/>
     </row>
-    <row r="73" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="P73" s="5"/>
     </row>
-    <row r="74" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>17</v>
       </c>
@@ -8718,7 +8718,7 @@
       </c>
       <c r="P74" s="5"/>
     </row>
-    <row r="75" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -8766,7 +8766,7 @@
       </c>
       <c r="P75" s="5"/>
     </row>
-    <row r="76" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>17</v>
       </c>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="P76" s="5"/>
     </row>
-    <row r="77" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>17</v>
       </c>
@@ -8862,7 +8862,7 @@
       </c>
       <c r="P77" s="5"/>
     </row>
-    <row r="78" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>17</v>
       </c>
@@ -8910,7 +8910,7 @@
       </c>
       <c r="P78" s="5"/>
     </row>
-    <row r="79" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -8958,7 +8958,7 @@
       </c>
       <c r="P79" s="5"/>
     </row>
-    <row r="80" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="P80" s="5"/>
     </row>
-    <row r="81" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>17</v>
       </c>
@@ -9054,7 +9054,7 @@
       </c>
       <c r="P81" s="5"/>
     </row>
-    <row r="82" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>17</v>
       </c>
@@ -9102,7 +9102,7 @@
       </c>
       <c r="P82" s="5"/>
     </row>
-    <row r="83" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>17</v>
       </c>
@@ -9150,7 +9150,7 @@
       </c>
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
@@ -9198,7 +9198,7 @@
       </c>
       <c r="P84" s="5"/>
     </row>
-    <row r="85" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>17</v>
       </c>
@@ -9246,7 +9246,7 @@
       </c>
       <c r="P85" s="5"/>
     </row>
-    <row r="86" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>17</v>
       </c>
@@ -9294,7 +9294,7 @@
       </c>
       <c r="P86" s="5"/>
     </row>
-    <row r="87" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>17</v>
       </c>
@@ -9342,7 +9342,7 @@
       </c>
       <c r="P87" s="5"/>
     </row>
-    <row r="88" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>17</v>
       </c>
@@ -9390,7 +9390,7 @@
       </c>
       <c r="P88" s="5"/>
     </row>
-    <row r="89" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>17</v>
       </c>
@@ -9438,7 +9438,7 @@
       </c>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>17</v>
       </c>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="P90" s="5"/>
     </row>
-    <row r="91" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>17</v>
       </c>
@@ -9534,7 +9534,7 @@
       </c>
       <c r="P91" s="5"/>
     </row>
-    <row r="92" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>17</v>
       </c>
@@ -9582,7 +9582,7 @@
       </c>
       <c r="P92" s="5"/>
     </row>
-    <row r="93" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>17</v>
       </c>
@@ -9630,7 +9630,7 @@
       </c>
       <c r="P93" s="5"/>
     </row>
-    <row r="94" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>17</v>
       </c>
@@ -9678,7 +9678,7 @@
       </c>
       <c r="P94" s="5"/>
     </row>
-    <row r="95" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>17</v>
       </c>
@@ -9726,7 +9726,7 @@
       </c>
       <c r="P95" s="5"/>
     </row>
-    <row r="96" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>17</v>
       </c>
@@ -9774,7 +9774,7 @@
       </c>
       <c r="P96" s="5"/>
     </row>
-    <row r="97" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>17</v>
       </c>
@@ -9822,7 +9822,7 @@
       </c>
       <c r="P97" s="5"/>
     </row>
-    <row r="98" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>17</v>
       </c>
@@ -9870,7 +9870,7 @@
       </c>
       <c r="P98" s="5"/>
     </row>
-    <row r="99" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>17</v>
       </c>
@@ -9918,7 +9918,7 @@
       </c>
       <c r="P99" s="5"/>
     </row>
-    <row r="100" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>17</v>
       </c>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="P100" s="5"/>
     </row>
-    <row r="101" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>17</v>
       </c>
@@ -10014,7 +10014,7 @@
       </c>
       <c r="P101" s="5"/>
     </row>
-    <row r="102" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>17</v>
       </c>
@@ -10062,7 +10062,7 @@
       </c>
       <c r="P102" s="5"/>
     </row>
-    <row r="103" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>17</v>
       </c>
@@ -10110,7 +10110,7 @@
       </c>
       <c r="P103" s="5"/>
     </row>
-    <row r="104" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>17</v>
       </c>
@@ -10158,7 +10158,7 @@
       </c>
       <c r="P104" s="5"/>
     </row>
-    <row r="105" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>17</v>
       </c>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="P105" s="5"/>
     </row>
-    <row r="106" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>17</v>
       </c>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="P106" s="5"/>
     </row>
-    <row r="107" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>17</v>
       </c>
@@ -10302,7 +10302,7 @@
       </c>
       <c r="P107" s="5"/>
     </row>
-    <row r="108" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>17</v>
       </c>
@@ -10350,7 +10350,7 @@
       </c>
       <c r="P108" s="5"/>
     </row>
-    <row r="109" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>17</v>
       </c>
@@ -10398,7 +10398,7 @@
       </c>
       <c r="P109" s="5"/>
     </row>
-    <row r="110" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>17</v>
       </c>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="P110" s="5"/>
     </row>
-    <row r="111" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>17</v>
       </c>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="P111" s="5"/>
     </row>
-    <row r="112" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>17</v>
       </c>
@@ -10542,7 +10542,7 @@
       </c>
       <c r="P112" s="5"/>
     </row>
-    <row r="113" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>17</v>
       </c>
@@ -10590,7 +10590,7 @@
       </c>
       <c r="P113" s="5"/>
     </row>
-    <row r="114" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>17</v>
       </c>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="P114" s="5"/>
     </row>
-    <row r="115" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>17</v>
       </c>
@@ -10686,7 +10686,7 @@
       </c>
       <c r="P115" s="5"/>
     </row>
-    <row r="116" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>17</v>
       </c>
@@ -10734,7 +10734,7 @@
       </c>
       <c r="P116" s="5"/>
     </row>
-    <row r="117" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>17</v>
       </c>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="P117" s="5"/>
     </row>
-    <row r="118" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>17</v>
       </c>
@@ -10830,7 +10830,7 @@
       </c>
       <c r="P118" s="5"/>
     </row>
-    <row r="119" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>17</v>
       </c>
@@ -10878,7 +10878,7 @@
       </c>
       <c r="P119" s="5"/>
     </row>
-    <row r="120" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>17</v>
       </c>
@@ -10926,7 +10926,7 @@
       </c>
       <c r="P120" s="5"/>
     </row>
-    <row r="121" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>17</v>
       </c>
@@ -10974,7 +10974,7 @@
       </c>
       <c r="P121" s="5"/>
     </row>
-    <row r="122" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="P122" s="5"/>
     </row>
-    <row r="123" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>17</v>
       </c>
@@ -11070,7 +11070,7 @@
       </c>
       <c r="P123" s="5"/>
     </row>
-    <row r="124" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>17</v>
       </c>
@@ -11118,7 +11118,7 @@
       </c>
       <c r="P124" s="5"/>
     </row>
-    <row r="125" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>17</v>
       </c>
@@ -11166,7 +11166,7 @@
       </c>
       <c r="P125" s="5"/>
     </row>
-    <row r="126" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>17</v>
       </c>
@@ -11214,7 +11214,7 @@
       </c>
       <c r="P126" s="5"/>
     </row>
-    <row r="127" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>17</v>
       </c>
@@ -11262,7 +11262,7 @@
       </c>
       <c r="P127" s="5"/>
     </row>
-    <row r="128" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>17</v>
       </c>
@@ -11310,7 +11310,7 @@
       </c>
       <c r="P128" s="5"/>
     </row>
-    <row r="129" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>17</v>
       </c>
@@ -11358,7 +11358,7 @@
       </c>
       <c r="P129" s="5"/>
     </row>
-    <row r="130" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>17</v>
       </c>
@@ -11406,7 +11406,7 @@
       </c>
       <c r="P130" s="5"/>
     </row>
-    <row r="131" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>17</v>
       </c>
@@ -11454,7 +11454,7 @@
       </c>
       <c r="P131" s="5"/>
     </row>
-    <row r="132" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>17</v>
       </c>
@@ -11502,7 +11502,7 @@
       </c>
       <c r="P132" s="5"/>
     </row>
-    <row r="133" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>17</v>
       </c>
@@ -11550,7 +11550,7 @@
       </c>
       <c r="P133" s="5"/>
     </row>
-    <row r="134" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>17</v>
       </c>
@@ -11598,7 +11598,7 @@
       </c>
       <c r="P134" s="5"/>
     </row>
-    <row r="135" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>17</v>
       </c>
@@ -11646,7 +11646,7 @@
       </c>
       <c r="P135" s="5"/>
     </row>
-    <row r="136" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>17</v>
       </c>
@@ -11694,7 +11694,7 @@
       </c>
       <c r="P136" s="5"/>
     </row>
-    <row r="137" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>17</v>
       </c>
@@ -11742,7 +11742,7 @@
       </c>
       <c r="P137" s="5"/>
     </row>
-    <row r="138" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>17</v>
       </c>
@@ -11790,7 +11790,7 @@
       </c>
       <c r="P138" s="5"/>
     </row>
-    <row r="139" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>17</v>
       </c>
@@ -11838,7 +11838,7 @@
       </c>
       <c r="P139" s="5"/>
     </row>
-    <row r="140" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>17</v>
       </c>
@@ -11886,7 +11886,7 @@
       </c>
       <c r="P140" s="5"/>
     </row>
-    <row r="141" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>17</v>
       </c>
@@ -11934,7 +11934,7 @@
       </c>
       <c r="P141" s="5"/>
     </row>
-    <row r="142" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>17</v>
       </c>
@@ -11982,7 +11982,7 @@
       </c>
       <c r="P142" s="5"/>
     </row>
-    <row r="143" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>17</v>
       </c>
@@ -12030,7 +12030,7 @@
       </c>
       <c r="P143" s="5"/>
     </row>
-    <row r="144" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>17</v>
       </c>
@@ -12078,7 +12078,7 @@
       </c>
       <c r="P144" s="5"/>
     </row>
-    <row r="145" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>17</v>
       </c>
@@ -12126,7 +12126,7 @@
       </c>
       <c r="P145" s="5"/>
     </row>
-    <row r="146" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>17</v>
       </c>
@@ -12174,7 +12174,7 @@
       </c>
       <c r="P146" s="5"/>
     </row>
-    <row r="147" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>17</v>
       </c>
@@ -12222,7 +12222,7 @@
       </c>
       <c r="P147" s="5"/>
     </row>
-    <row r="148" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>17</v>
       </c>
@@ -12270,7 +12270,7 @@
       </c>
       <c r="P148" s="5"/>
     </row>
-    <row r="149" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>17</v>
       </c>
@@ -12318,7 +12318,7 @@
       </c>
       <c r="P149" s="5"/>
     </row>
-    <row r="150" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>17</v>
       </c>
@@ -12366,7 +12366,7 @@
       </c>
       <c r="P150" s="5"/>
     </row>
-    <row r="151" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>17</v>
       </c>
@@ -12414,7 +12414,7 @@
       </c>
       <c r="P151" s="5"/>
     </row>
-    <row r="152" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>17</v>
       </c>
@@ -12462,7 +12462,7 @@
       </c>
       <c r="P152" s="5"/>
     </row>
-    <row r="153" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>17</v>
       </c>
@@ -12510,7 +12510,7 @@
       </c>
       <c r="P153" s="5"/>
     </row>
-    <row r="154" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>17</v>
       </c>
@@ -12558,7 +12558,7 @@
       </c>
       <c r="P154" s="5"/>
     </row>
-    <row r="155" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>17</v>
       </c>
@@ -12606,7 +12606,7 @@
       </c>
       <c r="P155" s="5"/>
     </row>
-    <row r="156" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>17</v>
       </c>
@@ -12654,7 +12654,7 @@
       </c>
       <c r="P156" s="5"/>
     </row>
-    <row r="157" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>17</v>
       </c>
@@ -12702,7 +12702,7 @@
       </c>
       <c r="P157" s="5"/>
     </row>
-    <row r="158" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>17</v>
       </c>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="P158" s="5"/>
     </row>
-    <row r="159" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>17</v>
       </c>
@@ -12798,7 +12798,7 @@
       </c>
       <c r="P159" s="5"/>
     </row>
-    <row r="160" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>17</v>
       </c>
@@ -12846,7 +12846,7 @@
       </c>
       <c r="P160" s="5"/>
     </row>
-    <row r="161" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>17</v>
       </c>
@@ -12894,7 +12894,7 @@
       </c>
       <c r="P161" s="5"/>
     </row>
-    <row r="162" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>17</v>
       </c>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="P162" s="5"/>
     </row>
-    <row r="163" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>17</v>
       </c>
@@ -12990,7 +12990,7 @@
       </c>
       <c r="P163" s="5"/>
     </row>
-    <row r="164" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>17</v>
       </c>
@@ -13038,7 +13038,7 @@
       </c>
       <c r="P164" s="5"/>
     </row>
-    <row r="165" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>17</v>
       </c>
@@ -13086,7 +13086,7 @@
       </c>
       <c r="P165" s="5"/>
     </row>
-    <row r="166" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>17</v>
       </c>
@@ -13134,7 +13134,7 @@
       </c>
       <c r="P166" s="5"/>
     </row>
-    <row r="167" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>17</v>
       </c>
@@ -13182,7 +13182,7 @@
       </c>
       <c r="P167" s="5"/>
     </row>
-    <row r="168" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>17</v>
       </c>
@@ -13230,7 +13230,7 @@
       </c>
       <c r="P168" s="5"/>
     </row>
-    <row r="169" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>17</v>
       </c>
@@ -13278,7 +13278,7 @@
       </c>
       <c r="P169" s="5"/>
     </row>
-    <row r="170" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>17</v>
       </c>
@@ -13326,7 +13326,7 @@
       </c>
       <c r="P170" s="5"/>
     </row>
-    <row r="171" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>17</v>
       </c>
@@ -13374,7 +13374,7 @@
       </c>
       <c r="P171" s="5"/>
     </row>
-    <row r="172" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>17</v>
       </c>
@@ -13422,7 +13422,7 @@
       </c>
       <c r="P172" s="5"/>
     </row>
-    <row r="173" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>17</v>
       </c>
@@ -13470,7 +13470,7 @@
       </c>
       <c r="P173" s="5"/>
     </row>
-    <row r="174" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>17</v>
       </c>
@@ -13518,7 +13518,7 @@
       </c>
       <c r="P174" s="5"/>
     </row>
-    <row r="175" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>17</v>
       </c>
@@ -13566,7 +13566,7 @@
       </c>
       <c r="P175" s="5"/>
     </row>
-    <row r="176" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>17</v>
       </c>
@@ -13614,7 +13614,7 @@
       </c>
       <c r="P176" s="5"/>
     </row>
-    <row r="177" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>17</v>
       </c>
@@ -13662,7 +13662,7 @@
       </c>
       <c r="P177" s="5"/>
     </row>
-    <row r="178" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>17</v>
       </c>
@@ -13710,7 +13710,7 @@
       </c>
       <c r="P178" s="5"/>
     </row>
-    <row r="179" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>17</v>
       </c>
@@ -13758,7 +13758,7 @@
       </c>
       <c r="P179" s="5"/>
     </row>
-    <row r="180" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>17</v>
       </c>
@@ -13806,7 +13806,7 @@
       </c>
       <c r="P180" s="5"/>
     </row>
-    <row r="181" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>17</v>
       </c>
@@ -13854,7 +13854,7 @@
       </c>
       <c r="P181" s="5"/>
     </row>
-    <row r="182" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>17</v>
       </c>
@@ -13902,7 +13902,7 @@
       </c>
       <c r="P182" s="5"/>
     </row>
-    <row r="183" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>17</v>
       </c>
@@ -13950,7 +13950,7 @@
       </c>
       <c r="P183" s="5"/>
     </row>
-    <row r="184" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>17</v>
       </c>
@@ -13998,7 +13998,7 @@
       </c>
       <c r="P184" s="5"/>
     </row>
-    <row r="185" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>17</v>
       </c>
@@ -14046,7 +14046,7 @@
       </c>
       <c r="P185" s="5"/>
     </row>
-    <row r="186" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>17</v>
       </c>
@@ -14094,7 +14094,7 @@
       </c>
       <c r="P186" s="5"/>
     </row>
-    <row r="187" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>17</v>
       </c>
@@ -14142,7 +14142,7 @@
       </c>
       <c r="P187" s="5"/>
     </row>
-    <row r="188" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>17</v>
       </c>
@@ -14190,7 +14190,7 @@
       </c>
       <c r="P188" s="5"/>
     </row>
-    <row r="189" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>17</v>
       </c>
@@ -14238,7 +14238,7 @@
       </c>
       <c r="P189" s="5"/>
     </row>
-    <row r="190" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>17</v>
       </c>
@@ -14286,7 +14286,7 @@
       </c>
       <c r="P190" s="5"/>
     </row>
-    <row r="191" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>17</v>
       </c>
@@ -14334,7 +14334,7 @@
       </c>
       <c r="P191" s="5"/>
     </row>
-    <row r="192" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>17</v>
       </c>
@@ -14382,7 +14382,7 @@
       </c>
       <c r="P192" s="5"/>
     </row>
-    <row r="193" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>17</v>
       </c>
@@ -14430,7 +14430,7 @@
       </c>
       <c r="P193" s="5"/>
     </row>
-    <row r="194" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>17</v>
       </c>
@@ -14478,7 +14478,7 @@
       </c>
       <c r="P194" s="5"/>
     </row>
-    <row r="195" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>17</v>
       </c>
@@ -14526,7 +14526,7 @@
       </c>
       <c r="P195" s="5"/>
     </row>
-    <row r="196" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>17</v>
       </c>
@@ -14574,7 +14574,7 @@
       </c>
       <c r="P196" s="5"/>
     </row>
-    <row r="197" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>17</v>
       </c>
@@ -14622,7 +14622,7 @@
       </c>
       <c r="P197" s="5"/>
     </row>
-    <row r="198" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>17</v>
       </c>
@@ -14670,7 +14670,7 @@
       </c>
       <c r="P198" s="5"/>
     </row>
-    <row r="199" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>17</v>
       </c>
@@ -14718,7 +14718,7 @@
       </c>
       <c r="P199" s="5"/>
     </row>
-    <row r="200" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>17</v>
       </c>
@@ -14766,7 +14766,7 @@
       </c>
       <c r="P200" s="5"/>
     </row>
-    <row r="201" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>17</v>
       </c>
@@ -14814,7 +14814,7 @@
       </c>
       <c r="P201" s="5"/>
     </row>
-    <row r="202" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>17</v>
       </c>
@@ -14862,7 +14862,7 @@
       </c>
       <c r="P202" s="5"/>
     </row>
-    <row r="203" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>17</v>
       </c>
@@ -14910,7 +14910,7 @@
       </c>
       <c r="P203" s="5"/>
     </row>
-    <row r="204" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>17</v>
       </c>
@@ -14958,7 +14958,7 @@
       </c>
       <c r="P204" s="5"/>
     </row>
-    <row r="205" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>17</v>
       </c>
@@ -15006,7 +15006,7 @@
       </c>
       <c r="P205" s="5"/>
     </row>
-    <row r="206" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>17</v>
       </c>
@@ -15054,7 +15054,7 @@
       </c>
       <c r="P206" s="5"/>
     </row>
-    <row r="207" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>17</v>
       </c>
@@ -15102,7 +15102,7 @@
       </c>
       <c r="P207" s="5"/>
     </row>
-    <row r="208" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>17</v>
       </c>
@@ -15150,7 +15150,7 @@
       </c>
       <c r="P208" s="5"/>
     </row>
-    <row r="209" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>17</v>
       </c>
@@ -15198,7 +15198,7 @@
       </c>
       <c r="P209" s="5"/>
     </row>
-    <row r="210" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>17</v>
       </c>
@@ -15246,7 +15246,7 @@
       </c>
       <c r="P210" s="5"/>
     </row>
-    <row r="211" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>17</v>
       </c>
@@ -15294,7 +15294,7 @@
       </c>
       <c r="P211" s="5"/>
     </row>
-    <row r="212" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>17</v>
       </c>
@@ -15342,7 +15342,7 @@
       </c>
       <c r="P212" s="5"/>
     </row>
-    <row r="213" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>17</v>
       </c>
@@ -15390,7 +15390,7 @@
       </c>
       <c r="P213" s="5"/>
     </row>
-    <row r="214" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>17</v>
       </c>
@@ -15438,7 +15438,7 @@
       </c>
       <c r="P214" s="5"/>
     </row>
-    <row r="215" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>17</v>
       </c>
@@ -15486,7 +15486,7 @@
       </c>
       <c r="P215" s="5"/>
     </row>
-    <row r="216" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>17</v>
       </c>
@@ -15534,7 +15534,7 @@
       </c>
       <c r="P216" s="5"/>
     </row>
-    <row r="217" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>17</v>
       </c>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="P217" s="5"/>
     </row>
-    <row r="218" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>17</v>
       </c>
@@ -15630,7 +15630,7 @@
       </c>
       <c r="P218" s="5"/>
     </row>
-    <row r="219" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>17</v>
       </c>
@@ -15678,7 +15678,7 @@
       </c>
       <c r="P219" s="5"/>
     </row>
-    <row r="220" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>17</v>
       </c>
@@ -15726,7 +15726,7 @@
       </c>
       <c r="P220" s="5"/>
     </row>
-    <row r="221" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>17</v>
       </c>
@@ -15774,7 +15774,7 @@
       </c>
       <c r="P221" s="5"/>
     </row>
-    <row r="222" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>17</v>
       </c>
@@ -15822,7 +15822,7 @@
       </c>
       <c r="P222" s="5"/>
     </row>
-    <row r="223" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>17</v>
       </c>
@@ -15870,7 +15870,7 @@
       </c>
       <c r="P223" s="5"/>
     </row>
-    <row r="224" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>17</v>
       </c>
@@ -15918,7 +15918,7 @@
       </c>
       <c r="P224" s="5"/>
     </row>
-    <row r="225" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>17</v>
       </c>
@@ -15966,7 +15966,7 @@
       </c>
       <c r="P225" s="5"/>
     </row>
-    <row r="226" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>17</v>
       </c>
@@ -16014,7 +16014,7 @@
       </c>
       <c r="P226" s="5"/>
     </row>
-    <row r="227" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>17</v>
       </c>
@@ -16062,7 +16062,7 @@
       </c>
       <c r="P227" s="5"/>
     </row>
-    <row r="228" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>17</v>
       </c>
@@ -16110,7 +16110,7 @@
       </c>
       <c r="P228" s="5"/>
     </row>
-    <row r="229" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>17</v>
       </c>
@@ -16158,7 +16158,7 @@
       </c>
       <c r="P229" s="5"/>
     </row>
-    <row r="230" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>17</v>
       </c>
@@ -16206,7 +16206,7 @@
       </c>
       <c r="P230" s="5"/>
     </row>
-    <row r="231" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>17</v>
       </c>
@@ -16254,7 +16254,7 @@
       </c>
       <c r="P231" s="5"/>
     </row>
-    <row r="232" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>17</v>
       </c>
@@ -16302,7 +16302,7 @@
       </c>
       <c r="P232" s="5"/>
     </row>
-    <row r="233" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>17</v>
       </c>
@@ -16350,7 +16350,7 @@
       </c>
       <c r="P233" s="5"/>
     </row>
-    <row r="234" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>17</v>
       </c>
@@ -16398,7 +16398,7 @@
       </c>
       <c r="P234" s="5"/>
     </row>
-    <row r="235" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>17</v>
       </c>
@@ -16446,7 +16446,7 @@
       </c>
       <c r="P235" s="5"/>
     </row>
-    <row r="236" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>17</v>
       </c>
@@ -16494,7 +16494,7 @@
       </c>
       <c r="P236" s="5"/>
     </row>
-    <row r="237" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>17</v>
       </c>
@@ -16542,7 +16542,7 @@
       </c>
       <c r="P237" s="5"/>
     </row>
-    <row r="238" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>17</v>
       </c>
@@ -16590,7 +16590,7 @@
       </c>
       <c r="P238" s="5"/>
     </row>
-    <row r="239" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>17</v>
       </c>
@@ -16638,7 +16638,7 @@
       </c>
       <c r="P239" s="5"/>
     </row>
-    <row r="240" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>17</v>
       </c>
@@ -16686,7 +16686,7 @@
       </c>
       <c r="P240" s="5"/>
     </row>
-    <row r="241" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>17</v>
       </c>
@@ -16734,7 +16734,7 @@
       </c>
       <c r="P241" s="5"/>
     </row>
-    <row r="242" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>17</v>
       </c>
@@ -16782,7 +16782,7 @@
       </c>
       <c r="P242" s="5"/>
     </row>
-    <row r="243" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>17</v>
       </c>
@@ -16830,7 +16830,7 @@
       </c>
       <c r="P243" s="5"/>
     </row>
-    <row r="244" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>17</v>
       </c>
@@ -16878,7 +16878,7 @@
       </c>
       <c r="P244" s="5"/>
     </row>
-    <row r="245" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>17</v>
       </c>
@@ -16926,7 +16926,7 @@
       </c>
       <c r="P245" s="5"/>
     </row>
-    <row r="246" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>17</v>
       </c>
@@ -16974,7 +16974,7 @@
       </c>
       <c r="P246" s="5"/>
     </row>
-    <row r="247" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>17</v>
       </c>
@@ -17022,7 +17022,7 @@
       </c>
       <c r="P247" s="5"/>
     </row>
-    <row r="248" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>17</v>
       </c>
@@ -17070,7 +17070,7 @@
       </c>
       <c r="P248" s="5"/>
     </row>
-    <row r="249" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>17</v>
       </c>
@@ -17118,7 +17118,7 @@
       </c>
       <c r="P249" s="5"/>
     </row>
-    <row r="250" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>17</v>
       </c>
@@ -17166,7 +17166,7 @@
       </c>
       <c r="P250" s="5"/>
     </row>
-    <row r="251" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>17</v>
       </c>
@@ -17214,7 +17214,7 @@
       </c>
       <c r="P251" s="5"/>
     </row>
-    <row r="252" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>17</v>
       </c>
@@ -17262,7 +17262,7 @@
       </c>
       <c r="P252" s="5"/>
     </row>
-    <row r="253" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>17</v>
       </c>
@@ -17310,7 +17310,7 @@
       </c>
       <c r="P253" s="5"/>
     </row>
-    <row r="254" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>17</v>
       </c>
@@ -17358,7 +17358,7 @@
       </c>
       <c r="P254" s="5"/>
     </row>
-    <row r="255" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>17</v>
       </c>
@@ -17406,7 +17406,7 @@
       </c>
       <c r="P255" s="5"/>
     </row>
-    <row r="256" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>17</v>
       </c>
@@ -17454,7 +17454,7 @@
       </c>
       <c r="P256" s="5"/>
     </row>
-    <row r="257" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>17</v>
       </c>
@@ -17502,7 +17502,7 @@
       </c>
       <c r="P257" s="5"/>
     </row>
-    <row r="258" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>17</v>
       </c>
@@ -17550,7 +17550,7 @@
       </c>
       <c r="P258" s="5"/>
     </row>
-    <row r="259" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>17</v>
       </c>
@@ -17598,7 +17598,7 @@
       </c>
       <c r="P259" s="5"/>
     </row>
-    <row r="260" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>17</v>
       </c>
@@ -17646,7 +17646,7 @@
       </c>
       <c r="P260" s="5"/>
     </row>
-    <row r="261" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>17</v>
       </c>
@@ -17694,7 +17694,7 @@
       </c>
       <c r="P261" s="5"/>
     </row>
-    <row r="262" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>17</v>
       </c>
@@ -17742,7 +17742,7 @@
       </c>
       <c r="P262" s="5"/>
     </row>
-    <row r="263" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>17</v>
       </c>
@@ -17790,7 +17790,7 @@
       </c>
       <c r="P263" s="5"/>
     </row>
-    <row r="264" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>17</v>
       </c>
@@ -17838,7 +17838,7 @@
       </c>
       <c r="P264" s="5"/>
     </row>
-    <row r="265" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>17</v>
       </c>
@@ -17886,7 +17886,7 @@
       </c>
       <c r="P265" s="5"/>
     </row>
-    <row r="266" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>17</v>
       </c>
@@ -17934,7 +17934,7 @@
       </c>
       <c r="P266" s="5"/>
     </row>
-    <row r="267" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>17</v>
       </c>
@@ -17982,7 +17982,7 @@
       </c>
       <c r="P267" s="5"/>
     </row>
-    <row r="268" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>17</v>
       </c>
@@ -18030,7 +18030,7 @@
       </c>
       <c r="P268" s="5"/>
     </row>
-    <row r="269" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>17</v>
       </c>
@@ -18078,7 +18078,7 @@
       </c>
       <c r="P269" s="5"/>
     </row>
-    <row r="270" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>17</v>
       </c>
@@ -18126,7 +18126,7 @@
       </c>
       <c r="P270" s="5"/>
     </row>
-    <row r="271" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>17</v>
       </c>
@@ -18174,7 +18174,7 @@
       </c>
       <c r="P271" s="5"/>
     </row>
-    <row r="272" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>17</v>
       </c>
@@ -18222,7 +18222,7 @@
       </c>
       <c r="P272" s="5"/>
     </row>
-    <row r="273" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>17</v>
       </c>
@@ -18270,7 +18270,7 @@
       </c>
       <c r="P273" s="5"/>
     </row>
-    <row r="274" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>17</v>
       </c>
@@ -18318,7 +18318,7 @@
       </c>
       <c r="P274" s="5"/>
     </row>
-    <row r="275" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>17</v>
       </c>
@@ -18366,7 +18366,7 @@
       </c>
       <c r="P275" s="5"/>
     </row>
-    <row r="276" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>17</v>
       </c>
@@ -18414,7 +18414,7 @@
       </c>
       <c r="P276" s="5"/>
     </row>
-    <row r="277" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>17</v>
       </c>
@@ -18462,7 +18462,7 @@
       </c>
       <c r="P277" s="5"/>
     </row>
-    <row r="278" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>17</v>
       </c>
@@ -18510,7 +18510,7 @@
       </c>
       <c r="P278" s="5"/>
     </row>
-    <row r="279" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>17</v>
       </c>
@@ -18558,7 +18558,7 @@
       </c>
       <c r="P279" s="5"/>
     </row>
-    <row r="280" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>17</v>
       </c>
@@ -18606,7 +18606,7 @@
       </c>
       <c r="P280" s="5"/>
     </row>
-    <row r="281" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>17</v>
       </c>
@@ -18654,7 +18654,7 @@
       </c>
       <c r="P281" s="5"/>
     </row>
-    <row r="282" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>17</v>
       </c>
@@ -18702,7 +18702,7 @@
       </c>
       <c r="P282" s="5"/>
     </row>
-    <row r="283" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>17</v>
       </c>
@@ -18750,7 +18750,7 @@
       </c>
       <c r="P283" s="5"/>
     </row>
-    <row r="284" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>17</v>
       </c>
@@ -18798,7 +18798,7 @@
       </c>
       <c r="P284" s="5"/>
     </row>
-    <row r="285" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>17</v>
       </c>
@@ -18846,7 +18846,7 @@
       </c>
       <c r="P285" s="5"/>
     </row>
-    <row r="286" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>17</v>
       </c>
@@ -18894,7 +18894,7 @@
       </c>
       <c r="P286" s="5"/>
     </row>
-    <row r="287" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>17</v>
       </c>
@@ -18942,7 +18942,7 @@
       </c>
       <c r="P287" s="5"/>
     </row>
-    <row r="288" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>17</v>
       </c>
@@ -18990,7 +18990,7 @@
       </c>
       <c r="P288" s="5"/>
     </row>
-    <row r="289" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>17</v>
       </c>
@@ -19038,7 +19038,7 @@
       </c>
       <c r="P289" s="5"/>
     </row>
-    <row r="290" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>17</v>
       </c>
@@ -19086,7 +19086,7 @@
       </c>
       <c r="P290" s="5"/>
     </row>
-    <row r="291" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>17</v>
       </c>
@@ -19134,7 +19134,7 @@
       </c>
       <c r="P291" s="5"/>
     </row>
-    <row r="292" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>17</v>
       </c>
@@ -19182,7 +19182,7 @@
       </c>
       <c r="P292" s="5"/>
     </row>
-    <row r="293" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>17</v>
       </c>
@@ -19230,7 +19230,7 @@
       </c>
       <c r="P293" s="5"/>
     </row>
-    <row r="294" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>17</v>
       </c>
@@ -19278,7 +19278,7 @@
       </c>
       <c r="P294" s="5"/>
     </row>
-    <row r="295" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>17</v>
       </c>
@@ -19326,7 +19326,7 @@
       </c>
       <c r="P295" s="5"/>
     </row>
-    <row r="296" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>17</v>
       </c>
@@ -19374,7 +19374,7 @@
       </c>
       <c r="P296" s="5"/>
     </row>
-    <row r="297" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>17</v>
       </c>
@@ -19422,7 +19422,7 @@
       </c>
       <c r="P297" s="5"/>
     </row>
-    <row r="298" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>17</v>
       </c>
@@ -19470,7 +19470,7 @@
       </c>
       <c r="P298" s="5"/>
     </row>
-    <row r="299" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>17</v>
       </c>
@@ -19518,7 +19518,7 @@
       </c>
       <c r="P299" s="5"/>
     </row>
-    <row r="300" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>17</v>
       </c>
@@ -19566,7 +19566,7 @@
       </c>
       <c r="P300" s="5"/>
     </row>
-    <row r="301" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>17</v>
       </c>
@@ -19614,7 +19614,7 @@
       </c>
       <c r="P301" s="5"/>
     </row>
-    <row r="302" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>17</v>
       </c>
@@ -19662,7 +19662,7 @@
       </c>
       <c r="P302" s="5"/>
     </row>
-    <row r="303" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>17</v>
       </c>
@@ -19710,7 +19710,7 @@
       </c>
       <c r="P303" s="5"/>
     </row>
-    <row r="304" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>17</v>
       </c>
@@ -19758,7 +19758,7 @@
       </c>
       <c r="P304" s="5"/>
     </row>
-    <row r="305" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>17</v>
       </c>
@@ -19806,7 +19806,7 @@
       </c>
       <c r="P305" s="5"/>
     </row>
-    <row r="306" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>17</v>
       </c>
@@ -19854,7 +19854,7 @@
       </c>
       <c r="P306" s="5"/>
     </row>
-    <row r="307" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-18-2021 22-06-24
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID_HN_CUARENTENA.xlsx
+++ b/datacovidhn/00 DATACOVID_HN_CUARENTENA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\OneDrive\CORONA VIRUS\DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{427060EC-FABC-4689-88EC-9238ABCB544F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0FC665FC-3440-41DA-9CEC-263A7F83650A}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{427060EC-FABC-4689-88EC-9238ABCB544F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C177D405-A436-4918-A6B0-9B78962F3534}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
@@ -4583,7 +4583,7 @@
     <t>https://www.google.com/maps/place/Municipio de Yorito + Departamento de Yoro + Honduras</t>
   </si>
   <si>
-    <t>Segmentando a la poblacion para poder circular conforme a la terminacion de los digitos de su tarjeta de identidad, pasaporte o carnet de residente para extranjeros, para que puedan abastecerse de insumos básicos,  con horario de 6:00 am a 8:00 pm.  De lunes a domingo, circulando dos digitos por día.</t>
+    <t>Segmentando a la poblacion para poder circular conforme a la terminacion de los digitos de su tarjeta de identidad, pasaporte o carnet de residente para extranjeros, para que puedan abastecerse de insumos básicos,  con horario de 5:00 am a 9:00 pm.  De lunes a domingo.</t>
   </si>
 </sst>
 </file>
@@ -5518,8 +5518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A9:Q307"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>